<commit_message>
created a new chart in Excel
</commit_message>
<xml_diff>
--- a/Intro_Excel_IsaacAdeyeye.xlsx
+++ b/Intro_Excel_IsaacAdeyeye.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rob Bentley\Dropbox\1 YouTubeing\2 Patreon\Documents to Upload to Patreon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/840dfa1d3898a61f/M4ACE_Projects/Project/my-first-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53583C8F-0B32-4D84-9EB4-CCC8FFA690BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{53583C8F-0B32-4D84-9EB4-CCC8FFA690BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8A609A5-88B1-44B1-A1EF-99CBF8DEF7BC}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10392" xr2:uid="{A2AB31B0-7DCA-432B-B293-18B64011FC4C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2AB31B0-7DCA-432B-B293-18B64011FC4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,16 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$82:$B$151</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$81</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$82:$C$151</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$81</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$D$82:$D$151</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$82:$B$151</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$C$81</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$C$82:$C$151</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$D$81</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$D$82:$D$151</definedName>
     <definedName name="TaxesOwed">Sheet1!$F$2:$F$71</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -32,7 +42,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="82">
   <si>
     <t>Julia</t>
   </si>
@@ -293,8 +302,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -336,15 +345,15 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3480,7 +3489,1332 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="sng" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1200" b="1" u="sng"/>
+              <a:t>Trend</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1200" b="1" u="sng" baseline="0"/>
+              <a:t> of Hourly wage with respect to Hours worked</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1200" b="1" u="sng"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="1" i="0" u="sng" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$81</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hours Worked</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$82:$B$151</c:f>
+              <c:strCache>
+                <c:ptCount val="70"/>
+                <c:pt idx="0">
+                  <c:v>Tanisha</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Riya</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Jayce</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Dangelo</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Derek</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Samuel</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jacinda</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Emma</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Adrienne</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Rogelio</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Jude</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Keegan</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Efrain</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Rosalinda</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Dangelo</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Ester</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Ellie</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Ariana</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Zayne</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Jaime</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Cortney</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Joshua</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Dante</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Kolton</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Clifford</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Freddy</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Glen</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Keisha</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Julia</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Ingrid</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Janay</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Macie</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Tanya</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Lilly</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Tre</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Dymond</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Alek</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Caden</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Raekwon</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Leandra</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>Jeff</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Marisela</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>James</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>Tanner</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Pranav</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Amelia</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>Danae</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>Kavon</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>Graciela</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>Andrea</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>Judah</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>Mari</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>Tianna</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>Jefferson</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>Audra</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>Kenan</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>Allan</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>Jordyn</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>Louis</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>Alvaro</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>Jayden</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>Dean Ling</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>Aubrie</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>Nestor</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>Lindsay</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>Keaton</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>Jerod</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>Phillip</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>Kerry</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>Anne</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$82:$D$151</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="70"/>
+                <c:pt idx="0">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6A8C-4A52-8F5E-746DCA155E2C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="835642224"/>
+        <c:axId val="835634320"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Hourly Wage</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$82:$B$151</c:f>
+              <c:strCache>
+                <c:ptCount val="70"/>
+                <c:pt idx="0">
+                  <c:v>Tanisha</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Riya</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Jayce</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Dangelo</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Derek</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Samuel</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jacinda</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Emma</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Adrienne</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Rogelio</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Jude</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Keegan</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Efrain</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Rosalinda</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Dangelo</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Ester</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Ellie</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Ariana</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Zayne</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Jaime</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Cortney</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Joshua</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Dante</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Kolton</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Clifford</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Freddy</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Glen</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Keisha</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Julia</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Ingrid</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Janay</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Macie</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Tanya</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Lilly</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Tre</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Dymond</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Alek</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Caden</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Raekwon</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Leandra</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>Jeff</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Marisela</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>James</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>Tanner</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Pranav</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Amelia</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>Danae</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>Kavon</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>Graciela</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>Andrea</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>Judah</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>Mari</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>Tianna</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>Jefferson</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>Audra</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>Kenan</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>Allan</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>Jordyn</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>Louis</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>Alvaro</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>Jayden</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>Dean Ling</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>Aubrie</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>Nestor</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>Lindsay</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>Keaton</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>Jerod</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>Phillip</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>Kerry</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>Anne</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$82:$C$151</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="70"/>
+                <c:pt idx="0">
+                  <c:v>10.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.75</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13.75</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13.75</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14.25</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6A8C-4A52-8F5E-746DCA155E2C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="967404704"/>
+        <c:axId val="967405120"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="967404704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="967405120"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="967405120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="967404704"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="835634320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="835642224"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="835642224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="835634320"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4025,20 +5359,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="322">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>363742</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:colOff>264682</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>521970</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4058,6 +5908,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>333894</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>139239</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>207819</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>138545</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80F7F0B7-5AC7-4795-AF0A-AEDB4A11AECD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4366,23 +6252,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I76"/>
+  <dimension ref="A1:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AB21" sqref="AB21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.3671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.89453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1015625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1015625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.47265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -4411,7 +6298,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4433,7 +6320,7 @@
         <v>157.60500000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4455,7 +6342,7 @@
         <v>173.60000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4477,7 +6364,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4499,7 +6386,7 @@
         <v>158.81250000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4521,7 +6408,7 @@
         <v>156.24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4543,7 +6430,7 @@
         <v>207.06000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4565,7 +6452,7 @@
         <v>154.96250000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4587,7 +6474,7 @@
         <v>74.865000000000009</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4609,7 +6496,7 @@
         <v>63.962500000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4631,7 +6518,7 @@
         <v>126.94500000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4653,7 +6540,7 @@
         <v>134.4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4675,7 +6562,7 @@
         <v>164.92000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4697,7 +6584,7 @@
         <v>106.10250000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4719,7 +6606,7 @@
         <v>62.160000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4741,7 +6628,7 @@
         <v>147.63000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4763,7 +6650,7 @@
         <v>157.08000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4785,7 +6672,7 @@
         <v>223.44000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4807,7 +6694,7 @@
         <v>209.44000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4829,7 +6716,7 @@
         <v>88.2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4851,7 +6738,7 @@
         <v>159.39000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4873,7 +6760,7 @@
         <v>65.52000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4895,7 +6782,7 @@
         <v>109.20000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4917,7 +6804,7 @@
         <v>262.08000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4939,7 +6826,7 @@
         <v>149.38000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4961,7 +6848,7 @@
         <v>445.76000000000005</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4983,7 +6870,7 @@
         <v>123.20000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5005,7 +6892,7 @@
         <v>152.88000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5027,7 +6914,7 @@
         <v>126.94500000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5049,7 +6936,7 @@
         <v>79.800000000000011</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5071,7 +6958,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5093,7 +6980,7 @@
         <v>94.39500000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5115,7 +7002,7 @@
         <v>106.92500000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5137,7 +7024,7 @@
         <v>155.4</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5159,7 +7046,7 @@
         <v>202.16000000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5181,7 +7068,7 @@
         <v>221.34000000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5203,7 +7090,7 @@
         <v>127.68</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5225,7 +7112,7 @@
         <v>112.00000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5247,7 +7134,7 @@
         <v>156.24</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5269,7 +7156,7 @@
         <v>77.035000000000011</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5291,7 +7178,7 @@
         <v>81.34</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5313,7 +7200,7 @@
         <v>141.12</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5335,7 +7222,7 @@
         <v>127.05000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5357,7 +7244,7 @@
         <v>121.80000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5379,7 +7266,7 @@
         <v>144.30500000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5401,7 +7288,7 @@
         <v>75.67</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5423,7 +7310,7 @@
         <v>62.160000000000004</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5445,7 +7332,7 @@
         <v>267.33000000000004</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5467,7 +7354,7 @@
         <v>133.28</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5489,7 +7376,7 @@
         <v>220.78000000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5511,7 +7398,7 @@
         <v>179.20000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5533,7 +7420,7 @@
         <v>147.42000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5555,7 +7442,7 @@
         <v>122.36000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5577,7 +7464,7 @@
         <v>139.965</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5599,7 +7486,7 @@
         <v>80.290000000000006</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5621,7 +7508,7 @@
         <v>93.240000000000009</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -5643,7 +7530,7 @@
         <v>143.22000000000003</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5665,7 +7552,7 @@
         <v>138.18</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5687,7 +7574,7 @@
         <v>157.08000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5709,7 +7596,7 @@
         <v>93.100000000000009</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5731,7 +7618,7 @@
         <v>164.22000000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5753,7 +7640,7 @@
         <v>95.76</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5775,7 +7662,7 @@
         <v>145.60000000000002</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -5797,7 +7684,7 @@
         <v>262.08000000000004</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -5819,7 +7706,7 @@
         <v>74.690000000000012</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -5841,7 +7728,7 @@
         <v>215.91500000000002</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -5863,7 +7750,7 @@
         <v>123.20000000000002</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -5885,7 +7772,7 @@
         <v>131.04000000000002</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -5907,7 +7794,7 @@
         <v>126.94500000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -5929,7 +7816,7 @@
         <v>58.52</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -5951,7 +7838,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C72" s="3" t="s">
         <v>76</v>
       </c>
@@ -5968,7 +7855,7 @@
         <v>9995.6150000000034</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C73" s="3" t="s">
         <v>77</v>
       </c>
@@ -5985,7 +7872,7 @@
         <v>142.79450000000006</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C74" s="3" t="s">
         <v>78</v>
       </c>
@@ -6002,7 +7889,7 @@
         <v>445.76000000000005</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C75" s="3" t="s">
         <v>79</v>
       </c>
@@ -6019,7 +7906,7 @@
         <v>58.52</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C76" s="3" t="s">
         <v>80</v>
       </c>
@@ -6036,7 +7923,791 @@
         <v>70</v>
       </c>
     </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B81" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B82" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="2">
+        <v>10.75</v>
+      </c>
+      <c r="D82">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B83" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C83" s="2">
+        <v>11</v>
+      </c>
+      <c r="D83">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B84" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C84" s="2">
+        <v>11</v>
+      </c>
+      <c r="D84">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B85" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" s="2">
+        <v>11</v>
+      </c>
+      <c r="D85">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B86" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C86" s="2">
+        <v>11</v>
+      </c>
+      <c r="D86">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B87" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C87" s="2">
+        <v>11</v>
+      </c>
+      <c r="D87">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B88" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C88" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="D88">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B89" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C89" s="2">
+        <v>11.75</v>
+      </c>
+      <c r="D89">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B90" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" s="2">
+        <v>11.75</v>
+      </c>
+      <c r="D90">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B91" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C91" s="2">
+        <v>11.75</v>
+      </c>
+      <c r="D91">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B92" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C92" s="2">
+        <v>11.75</v>
+      </c>
+      <c r="D92">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B93" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C93" s="2">
+        <v>12</v>
+      </c>
+      <c r="D93">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B94" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C94" s="2">
+        <v>12</v>
+      </c>
+      <c r="D94">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B95" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C95" s="2">
+        <v>12</v>
+      </c>
+      <c r="D95">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B96" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C96" s="2">
+        <v>12</v>
+      </c>
+      <c r="D96">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B97" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C97" s="2">
+        <v>12</v>
+      </c>
+      <c r="D97">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B98" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C98" s="2">
+        <v>12</v>
+      </c>
+      <c r="D98">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B99" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C99" s="2">
+        <v>12</v>
+      </c>
+      <c r="D99">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B100" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C100" s="2">
+        <v>12</v>
+      </c>
+      <c r="D100">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B101" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C101" s="2">
+        <v>12</v>
+      </c>
+      <c r="D101">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B102" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C102" s="2">
+        <v>12</v>
+      </c>
+      <c r="D102">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B103" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C103" s="2">
+        <v>12</v>
+      </c>
+      <c r="D103">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B104" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C104" s="2">
+        <v>12</v>
+      </c>
+      <c r="D104">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B105" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C105" s="2">
+        <v>13</v>
+      </c>
+      <c r="D105">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B106" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C106" s="2">
+        <v>13.75</v>
+      </c>
+      <c r="D106">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B107" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C107" s="2">
+        <v>13.75</v>
+      </c>
+      <c r="D107">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B108" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C108" s="2">
+        <v>14</v>
+      </c>
+      <c r="D108">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B109" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C109" s="2">
+        <v>14</v>
+      </c>
+      <c r="D109">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B110" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C110" s="2">
+        <v>14.25</v>
+      </c>
+      <c r="D110">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B111" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C111" s="2">
+        <v>15</v>
+      </c>
+      <c r="D111">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B112" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C112" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="D112">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B113" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C113" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="D113">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B114" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C114" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="D114">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B115" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C115" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="D115">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B116" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C116" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="D116">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B117" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C117" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="D117">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B118" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C118" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="D118">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B119" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C119" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="D119">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B120" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C120" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="D120">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B121" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C121" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="D121">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B122" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C122" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="D122">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B123" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C123" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="D123">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B124" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C124" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="D124">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B125" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C125" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="D125">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B126" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C126" s="2">
+        <v>16</v>
+      </c>
+      <c r="D126">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B127" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C127" s="2">
+        <v>16</v>
+      </c>
+      <c r="D127">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B128" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C128" s="2">
+        <v>16</v>
+      </c>
+      <c r="D128">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B129" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C129" s="2">
+        <v>16</v>
+      </c>
+      <c r="D129">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B130" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C130" s="2">
+        <v>16</v>
+      </c>
+      <c r="D130">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B131" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C131" s="2">
+        <v>16.5</v>
+      </c>
+      <c r="D131">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B132" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C132" s="2">
+        <v>17</v>
+      </c>
+      <c r="D132">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B133" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C133" s="2">
+        <v>17</v>
+      </c>
+      <c r="D133">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B134" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C134" s="2">
+        <v>17</v>
+      </c>
+      <c r="D134">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B135" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C135" s="2">
+        <v>17</v>
+      </c>
+      <c r="D135">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B136" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C136" s="2">
+        <v>17</v>
+      </c>
+      <c r="D136">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B137" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C137" s="2">
+        <v>18</v>
+      </c>
+      <c r="D137">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B138" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C138" s="2">
+        <v>18</v>
+      </c>
+      <c r="D138">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B139" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C139" s="2">
+        <v>18</v>
+      </c>
+      <c r="D139">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B140" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C140" s="2">
+        <v>18</v>
+      </c>
+      <c r="D140">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B141" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C141" s="2">
+        <v>18</v>
+      </c>
+      <c r="D141">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B142" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C142" s="2">
+        <v>19</v>
+      </c>
+      <c r="D142">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B143" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C143" s="2">
+        <v>19</v>
+      </c>
+      <c r="D143">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B144" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C144" s="2">
+        <v>19</v>
+      </c>
+      <c r="D144">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B145" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C145" s="2">
+        <v>19</v>
+      </c>
+      <c r="D145">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B146" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C146" s="2">
+        <v>19</v>
+      </c>
+      <c r="D146">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B147" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C147" s="2">
+        <v>19</v>
+      </c>
+      <c r="D147">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B148" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C148" s="2">
+        <v>19</v>
+      </c>
+      <c r="D148">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B149" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C149" s="2">
+        <v>19</v>
+      </c>
+      <c r="D149">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B150" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C150" s="2">
+        <v>22</v>
+      </c>
+      <c r="D150">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B151" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C151" s="2">
+        <v>32</v>
+      </c>
+      <c r="D151">
+        <v>199</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B82:D151">
+    <sortCondition ref="C81:C151"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="45" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -6049,7 +8720,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6061,7 +8732,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>